<commit_message>
Fixed unknown in xlm (rest has not changed)
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/tokenizer_stats_pos_mbert.xlsx
+++ b/data_exploration/acl/tables/tokenizer_stats_pos_mbert.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aturt\Documents\typology_of_crosslingual\data_exploration\acl\tables\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -129,8 +124,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,19 +188,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -247,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,10 +266,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,7 +300,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,16 +475,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,145 +532,145 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2">
-        <v>37.774477447744772</v>
+        <v>37.77447744774477</v>
       </c>
       <c r="C2">
-        <v>44.255467862655443</v>
+        <v>44.25546786265544</v>
       </c>
       <c r="D2">
         <v>1.849462678743047</v>
       </c>
       <c r="E2">
-        <v>149.32013201320129</v>
+        <v>149.3201320132013</v>
       </c>
       <c r="F2">
-        <v>3.9529370649736442</v>
+        <v>3.952937064973644</v>
       </c>
       <c r="G2">
-        <v>47.414705882352941</v>
+        <v>47.41470588235294</v>
       </c>
       <c r="H2">
-        <v>45.282550710253702</v>
+        <v>45.2825507102537</v>
       </c>
       <c r="I2">
-        <v>1.8853669127225361</v>
+        <v>1.885366912722536</v>
       </c>
       <c r="J2">
         <v>193.4014705882353</v>
       </c>
       <c r="K2">
-        <v>4.0789343092860246</v>
+        <v>4.078934309286025</v>
       </c>
       <c r="L2">
-        <v>42.006584362139918</v>
+        <v>42.00658436213992</v>
       </c>
       <c r="M2">
-        <v>45.246678945099731</v>
+        <v>45.24667894509973</v>
       </c>
       <c r="N2">
         <v>1.881805713390023</v>
       </c>
       <c r="O2">
-        <v>171.35489711934159</v>
+        <v>171.3548971193416</v>
       </c>
       <c r="P2">
-        <v>4.0792389983933539</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>4.079238998393354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3">
-        <v>17.110294117647062</v>
+        <v>17.11029411764706</v>
       </c>
       <c r="C3">
-        <v>58.616244091104427</v>
+        <v>58.61624409110443</v>
       </c>
       <c r="D3">
-        <v>1.9411259131929519</v>
+        <v>1.941125913192952</v>
       </c>
       <c r="E3">
-        <v>58.897058823529413</v>
+        <v>58.89705882352941</v>
       </c>
       <c r="F3">
-        <v>3.4422002578427162</v>
+        <v>3.442200257842716</v>
       </c>
       <c r="G3">
         <v>15.69230769230769</v>
       </c>
       <c r="H3">
-        <v>61.541889483065958</v>
+        <v>61.54188948306596</v>
       </c>
       <c r="I3">
-        <v>2.0022281639928701</v>
+        <v>2.00222816399287</v>
       </c>
       <c r="J3">
         <v>55.67832167832168</v>
       </c>
       <c r="K3">
-        <v>3.5481283422459891</v>
+        <v>3.548128342245989</v>
       </c>
       <c r="L3">
-        <v>16.248746238716151</v>
+        <v>16.24874623871615</v>
       </c>
       <c r="M3">
-        <v>59.129629629629633</v>
+        <v>59.12962962962963</v>
       </c>
       <c r="N3">
         <v>1.941111111111111</v>
       </c>
       <c r="O3">
-        <v>56.297893681043128</v>
+        <v>56.29789368104313</v>
       </c>
       <c r="P3">
-        <v>3.4647530864197531</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3.464753086419753</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4">
-        <v>19.131062167733539</v>
+        <v>19.13106216773354</v>
       </c>
       <c r="C4">
-        <v>23.493883661976621</v>
+        <v>23.49388366197662</v>
       </c>
       <c r="D4">
-        <v>1.4255434381929439</v>
+        <v>1.425543438192944</v>
       </c>
       <c r="E4">
-        <v>98.551535206683297</v>
+        <v>98.5515352066833</v>
       </c>
       <c r="F4">
-        <v>5.1513885817014593</v>
+        <v>5.151388581701459</v>
       </c>
       <c r="G4">
-        <v>19.664553876157971</v>
+        <v>19.66455387615797</v>
       </c>
       <c r="H4">
-        <v>23.726128687449719</v>
+        <v>23.72612868744972</v>
       </c>
       <c r="I4">
         <v>1.418785194000904</v>
       </c>
       <c r="J4">
-        <v>100.81244921176661</v>
+        <v>100.8124492117666</v>
       </c>
       <c r="K4">
-        <v>5.1266074911567321</v>
+        <v>5.126607491156732</v>
       </c>
       <c r="L4">
-        <v>19.816623799275629</v>
+        <v>19.81662379927563</v>
       </c>
       <c r="M4">
-        <v>23.566160256299892</v>
+        <v>23.56616025629989</v>
       </c>
       <c r="N4">
         <v>1.426738255460213</v>
@@ -696,77 +679,77 @@
         <v>102.0217048973807</v>
       </c>
       <c r="P4">
-        <v>5.1482889280620032</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>5.148288928062003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5">
-        <v>27.315136476426801</v>
+        <v>27.3151364764268</v>
       </c>
       <c r="C5">
-        <v>37.472747093023258</v>
+        <v>37.47274709302326</v>
       </c>
       <c r="D5">
-        <v>2.2753452034883721</v>
+        <v>2.275345203488372</v>
       </c>
       <c r="E5">
-        <v>130.81885856079401</v>
+        <v>130.818858560794</v>
       </c>
       <c r="F5">
-        <v>4.7892441860465116</v>
+        <v>4.789244186046512</v>
       </c>
       <c r="G5">
-        <v>24.348684210526319</v>
+        <v>24.34868421052632</v>
       </c>
       <c r="H5">
-        <v>39.250652976672967</v>
+        <v>39.25065297667297</v>
       </c>
       <c r="I5">
-        <v>2.3520670089165092</v>
+        <v>2.352067008916509</v>
       </c>
       <c r="J5">
         <v>117.7850877192982</v>
       </c>
       <c r="K5">
-        <v>4.8374313248671532</v>
+        <v>4.837431324867153</v>
       </c>
       <c r="L5">
         <v>26.52406738868833</v>
       </c>
       <c r="M5">
-        <v>39.255495315654557</v>
+        <v>39.25549531565456</v>
       </c>
       <c r="N5">
-        <v>2.3482521606968669</v>
+        <v>2.348252160696867</v>
       </c>
       <c r="O5">
-        <v>129.09145607701561</v>
+        <v>129.0914560770156</v>
       </c>
       <c r="P5">
-        <v>4.8669555157316884</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>4.866955515731688</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6">
-        <v>32.214026602176538</v>
+        <v>32.21402660217654</v>
       </c>
       <c r="C6">
-        <v>18.679854359821331</v>
+        <v>18.67985435982133</v>
       </c>
       <c r="D6">
-        <v>1.2813520513494241</v>
+        <v>1.281352051349424</v>
       </c>
       <c r="E6">
-        <v>140.57496977025389</v>
+        <v>140.5749697702539</v>
       </c>
       <c r="F6">
-        <v>4.3637813895874782</v>
+        <v>4.363781389587478</v>
       </c>
       <c r="G6">
         <v>31.09355026147589</v>
@@ -775,7 +758,7 @@
         <v>18.4089550007475</v>
       </c>
       <c r="I6">
-        <v>1.2784609059650169</v>
+        <v>1.278460905965017</v>
       </c>
       <c r="J6">
         <v>135.9529343404997</v>
@@ -784,80 +767,80 @@
         <v>4.372383764389296</v>
       </c>
       <c r="L6">
-        <v>31.564557846906681</v>
+        <v>31.56455784690668</v>
       </c>
       <c r="M6">
-        <v>18.325430590590681</v>
+        <v>18.32543059059068</v>
       </c>
       <c r="N6">
-        <v>1.2759212545760981</v>
+        <v>1.275921254576098</v>
       </c>
       <c r="O6">
-        <v>138.23893743446351</v>
+        <v>138.2389374344635</v>
       </c>
       <c r="P6">
-        <v>4.3795619791332161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>4.379561979133216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7">
-        <v>13.728031145717461</v>
+        <v>13.72803114571746</v>
       </c>
       <c r="C7">
-        <v>52.315358748936511</v>
+        <v>52.31535874893651</v>
       </c>
       <c r="D7">
         <v>1.87238180123972</v>
       </c>
       <c r="E7">
-        <v>75.126807563959957</v>
+        <v>75.12680756395996</v>
       </c>
       <c r="F7">
-        <v>5.4725114451241748</v>
+        <v>5.472511445124175</v>
       </c>
       <c r="G7">
-        <v>13.892162312395779</v>
+        <v>13.89216231239578</v>
       </c>
       <c r="H7">
-        <v>52.632842509603073</v>
+        <v>52.63284250960307</v>
       </c>
       <c r="I7">
-        <v>1.8781209987195899</v>
+        <v>1.87812099871959</v>
       </c>
       <c r="J7">
-        <v>76.550305725403007</v>
+        <v>76.55030572540301</v>
       </c>
       <c r="K7">
-        <v>5.5103233034571062</v>
+        <v>5.510323303457106</v>
       </c>
       <c r="L7">
-        <v>13.856745737583401</v>
+        <v>13.8567457375834</v>
       </c>
       <c r="M7">
-        <v>52.177983442778618</v>
+        <v>52.17798344277862</v>
       </c>
       <c r="N7">
-        <v>1.8737612175843581</v>
+        <v>1.873761217584358</v>
       </c>
       <c r="O7">
-        <v>75.742772424017787</v>
+        <v>75.74277242401779</v>
       </c>
       <c r="P7">
-        <v>5.4661299166789261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>5.466129916678926</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8">
-        <v>14.049120234604111</v>
+        <v>14.04912023460411</v>
       </c>
       <c r="C8">
-        <v>53.290194645932267</v>
+        <v>53.29019464593227</v>
       </c>
       <c r="D8">
         <v>2.124928247142932</v>
@@ -866,166 +849,166 @@
         <v>86.99120234604105</v>
       </c>
       <c r="F8">
-        <v>6.1919323696707194</v>
+        <v>6.191932369670719</v>
       </c>
       <c r="G8">
         <v>14.16720257234727</v>
       </c>
       <c r="H8">
-        <v>52.401270994098958</v>
+        <v>52.40127099409896</v>
       </c>
       <c r="I8">
         <v>2.117884702678166</v>
       </c>
       <c r="J8">
-        <v>86.239228295819942</v>
+        <v>86.23922829581994</v>
       </c>
       <c r="K8">
-        <v>6.0872446663640494</v>
+        <v>6.087244666364049</v>
       </c>
       <c r="L8">
         <v>13.97732667594336</v>
       </c>
       <c r="M8">
-        <v>53.654522988270159</v>
+        <v>53.65452298827016</v>
       </c>
       <c r="N8">
-        <v>2.1453024988141318</v>
+        <v>2.145302498814132</v>
       </c>
       <c r="O8">
-        <v>86.903167717115494</v>
+        <v>86.90316771711549</v>
       </c>
       <c r="P8">
-        <v>6.2174384080674159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>6.217438408067416</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9">
-        <v>31.493801652892561</v>
+        <v>31.49380165289256</v>
       </c>
       <c r="C9">
-        <v>39.021190054451218</v>
+        <v>39.02119005445122</v>
       </c>
       <c r="D9">
-        <v>1.7097028144066131</v>
+        <v>1.709702814406613</v>
       </c>
       <c r="E9">
         <v>103.2479338842975</v>
       </c>
       <c r="F9">
-        <v>3.2783572787509021</v>
+        <v>3.278357278750902</v>
       </c>
       <c r="G9">
-        <v>33.281059063136453</v>
+        <v>33.28105906313645</v>
       </c>
       <c r="H9">
-        <v>40.848173306407197</v>
+        <v>40.8481733064072</v>
       </c>
       <c r="I9">
-        <v>1.7477510556269511</v>
+        <v>1.747751055626951</v>
       </c>
       <c r="J9">
-        <v>109.09775967413439</v>
+        <v>109.0977596741344</v>
       </c>
       <c r="K9">
-        <v>3.2780735573098339</v>
+        <v>3.278073557309834</v>
       </c>
       <c r="L9">
-        <v>35.668956306048457</v>
+        <v>35.66895630604846</v>
       </c>
       <c r="M9">
-        <v>38.775870461803457</v>
+        <v>38.77587046180346</v>
       </c>
       <c r="N9">
-        <v>1.7006595663872559</v>
+        <v>1.700659566387256</v>
       </c>
       <c r="O9">
         <v>114.2289639381797</v>
       </c>
       <c r="P9">
-        <v>3.2024756473967719</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3.202475647396772</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10">
-        <v>22.744186046511629</v>
+        <v>22.74418604651163</v>
       </c>
       <c r="C10">
-        <v>25.247758376592731</v>
+        <v>25.24775837659273</v>
       </c>
       <c r="D10">
-        <v>1.3992449268522891</v>
+        <v>1.399244926852289</v>
       </c>
       <c r="E10">
-        <v>116.47942754919499</v>
+        <v>116.479427549195</v>
       </c>
       <c r="F10">
-        <v>5.1212836243511086</v>
+        <v>5.121283624351109</v>
       </c>
       <c r="G10">
         <v>21.32315978456014</v>
       </c>
       <c r="H10">
-        <v>24.854761303359439</v>
+        <v>24.85476130335944</v>
       </c>
       <c r="I10">
-        <v>1.3932811315988891</v>
+        <v>1.393281131598889</v>
       </c>
       <c r="J10">
         <v>109.4955116696589</v>
       </c>
       <c r="K10">
-        <v>5.1350509387892567</v>
+        <v>5.135050938789257</v>
       </c>
       <c r="L10">
-        <v>21.962028143846329</v>
+        <v>21.96202814384633</v>
       </c>
       <c r="M10">
         <v>24.86066474106017</v>
       </c>
       <c r="N10">
-        <v>1.3933831007688871</v>
+        <v>1.393383100768887</v>
       </c>
       <c r="O10">
-        <v>112.72258208621849</v>
+        <v>112.7225820862185</v>
       </c>
       <c r="P10">
-        <v>5.1326125869574062</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>5.132612586957406</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11">
-        <v>30.968063872255492</v>
+        <v>30.96806387225549</v>
       </c>
       <c r="C11">
-        <v>9.2555591363196914</v>
+        <v>9.255559136319691</v>
       </c>
       <c r="D11">
         <v>1.144763132452465</v>
       </c>
       <c r="E11">
-        <v>39.870259481037927</v>
+        <v>39.87025948103793</v>
       </c>
       <c r="F11">
         <v>1.287463744763133</v>
       </c>
       <c r="G11">
-        <v>30.567219152854509</v>
+        <v>30.56721915285451</v>
       </c>
       <c r="H11">
         <v>10.56151343535366</v>
       </c>
       <c r="I11">
-        <v>1.1588745632003861</v>
+        <v>1.158874563200386</v>
       </c>
       <c r="J11">
         <v>39.7255985267035</v>
@@ -1034,22 +1017,22 @@
         <v>1.299614411374864</v>
       </c>
       <c r="L11">
-        <v>30.357051373274508</v>
+        <v>30.35705137327451</v>
       </c>
       <c r="M11">
-        <v>9.3789113956093928</v>
+        <v>9.378911395609393</v>
       </c>
       <c r="N11">
         <v>1.148800622541827</v>
       </c>
       <c r="O11">
-        <v>39.571936815141598</v>
+        <v>39.5719368151416</v>
       </c>
       <c r="P11">
         <v>1.303550082271153</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1057,49 +1040,49 @@
         <v>12.29380445304937</v>
       </c>
       <c r="C12">
-        <v>68.443639513366676</v>
+        <v>68.44363951336668</v>
       </c>
       <c r="D12">
-        <v>2.3659199181070121</v>
+        <v>2.365919918107012</v>
       </c>
       <c r="E12">
-        <v>36.135527589545013</v>
+        <v>36.13552758954501</v>
       </c>
       <c r="F12">
-        <v>2.9393283200125988</v>
+        <v>2.939328320012599</v>
       </c>
       <c r="G12">
-        <v>12.523393091386099</v>
+        <v>12.5233930913861</v>
       </c>
       <c r="H12">
-        <v>65.797283614398935</v>
+        <v>65.79728361439894</v>
       </c>
       <c r="I12">
-        <v>2.2867916623022939</v>
+        <v>2.286791662302294</v>
       </c>
       <c r="J12">
-        <v>36.317446436379527</v>
+        <v>36.31744643637953</v>
       </c>
       <c r="K12">
-        <v>2.8999685765161831</v>
+        <v>2.899968576516183</v>
       </c>
       <c r="L12">
-        <v>12.948196436332029</v>
+        <v>12.94819643633203</v>
       </c>
       <c r="M12">
-        <v>66.611509777201974</v>
+        <v>66.61150977720197</v>
       </c>
       <c r="N12">
         <v>2.258825661714853</v>
       </c>
       <c r="O12">
-        <v>36.712863972186007</v>
+        <v>36.71286397218601</v>
       </c>
       <c r="P12">
-        <v>2.8353650759554001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2.8353650759554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1107,34 +1090,34 @@
         <v>27.86374133949192</v>
       </c>
       <c r="C13">
-        <v>47.443016991297142</v>
+        <v>47.44301699129714</v>
       </c>
       <c r="D13">
         <v>1.861334438458351</v>
       </c>
       <c r="E13">
-        <v>108.17321016166279</v>
+        <v>108.1732101616628</v>
       </c>
       <c r="F13">
-        <v>3.8822213012847082</v>
+        <v>3.882221301284708</v>
       </c>
       <c r="G13">
-        <v>24.897683397683402</v>
+        <v>24.8976833976834</v>
       </c>
       <c r="H13">
-        <v>49.050166705435373</v>
+        <v>49.05016670543537</v>
       </c>
       <c r="I13">
-        <v>1.9135457858416689</v>
+        <v>1.913545785841669</v>
       </c>
       <c r="J13">
-        <v>94.882239382239376</v>
+        <v>94.88223938223938</v>
       </c>
       <c r="K13">
-        <v>3.8108862526168878</v>
+        <v>3.810886252616888</v>
       </c>
       <c r="L13">
-        <v>23.825467497773818</v>
+        <v>23.82546749777382</v>
       </c>
       <c r="M13">
         <v>46.63253102107938</v>
@@ -1146,98 +1129,98 @@
         <v>91.67764915405165</v>
       </c>
       <c r="P13">
-        <v>3.8478845866347742</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3.847884586634774</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>28</v>
       </c>
       <c r="B14">
-        <v>15.365296803652971</v>
+        <v>15.36529680365297</v>
       </c>
       <c r="C14">
-        <v>27.940024314467109</v>
+        <v>27.94002431446711</v>
       </c>
       <c r="D14">
-        <v>1.4781845197892749</v>
+        <v>1.478184519789275</v>
       </c>
       <c r="E14">
-        <v>67.782897467828974</v>
+        <v>67.78289746782897</v>
       </c>
       <c r="F14">
-        <v>4.4114277995407267</v>
+        <v>4.411427799540727</v>
       </c>
       <c r="G14">
         <v>15.73336771531717</v>
       </c>
       <c r="H14">
-        <v>27.554331792703309</v>
+        <v>27.55433179270331</v>
       </c>
       <c r="I14">
-        <v>1.4887730684760869</v>
+        <v>1.488773068476087</v>
       </c>
       <c r="J14">
         <v>69.26250644662197</v>
       </c>
       <c r="K14">
-        <v>4.4022683318582621</v>
+        <v>4.402268331858262</v>
       </c>
       <c r="L14">
-        <v>15.847094801223241</v>
+        <v>15.84709480122324</v>
       </c>
       <c r="M14">
-        <v>26.985639392769841</v>
+        <v>26.98563939276984</v>
       </c>
       <c r="N14">
-        <v>1.4602309275697929</v>
+        <v>1.460230927569793</v>
       </c>
       <c r="O14">
-        <v>69.503249235474001</v>
+        <v>69.503249235474</v>
       </c>
       <c r="P14">
-        <v>4.3858669432651487</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>4.385866943265149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>29</v>
       </c>
       <c r="B15">
-        <v>11.735849056603771</v>
+        <v>11.73584905660377</v>
       </c>
       <c r="C15">
-        <v>48.569131832797432</v>
+        <v>48.56913183279743</v>
       </c>
       <c r="D15">
         <v>1.9991961414791</v>
       </c>
       <c r="E15">
-        <v>60.043396226415098</v>
+        <v>60.0433962264151</v>
       </c>
       <c r="F15">
-        <v>5.1162379421221864</v>
+        <v>5.116237942122186</v>
       </c>
       <c r="G15">
-        <v>12.278982092365689</v>
+        <v>12.27898209236569</v>
       </c>
       <c r="H15">
-        <v>50.391464537918331</v>
+        <v>50.39146453791833</v>
       </c>
       <c r="I15">
-        <v>2.0333896223518582</v>
+        <v>2.033389622351858</v>
       </c>
       <c r="J15">
-        <v>63.353440150801127</v>
+        <v>63.35344015080113</v>
       </c>
       <c r="K15">
-        <v>5.1595026097635861</v>
+        <v>5.159502609763586</v>
       </c>
       <c r="L15">
-        <v>9.4997052929388186</v>
+        <v>9.499705292938819</v>
       </c>
       <c r="M15">
-        <v>47.581465763283937</v>
+        <v>47.58146576328394</v>
       </c>
       <c r="N15">
         <v>1.929367383912838</v>
@@ -1246,30 +1229,30 @@
         <v>42.87999528468702</v>
       </c>
       <c r="P15">
-        <v>4.5138237410964681</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>4.513823741096468</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="G16">
-        <v>22.425999999999998</v>
+        <v>22.426</v>
       </c>
       <c r="H16">
-        <v>76.576295371443862</v>
+        <v>76.57629537144386</v>
       </c>
       <c r="I16">
-        <v>3.0957816819762769</v>
+        <v>3.095781681976277</v>
       </c>
       <c r="J16">
-        <v>96.664000000000001</v>
+        <v>96.664</v>
       </c>
       <c r="K16">
         <v>4.310354053330955</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1277,31 +1260,31 @@
         <v>10.88663967611336</v>
       </c>
       <c r="C17">
-        <v>53.253997768687242</v>
+        <v>53.25399776868724</v>
       </c>
       <c r="D17">
         <v>1.978988471550762</v>
       </c>
       <c r="E17">
-        <v>55.164979757085021</v>
+        <v>55.16497975708502</v>
       </c>
       <c r="F17">
-        <v>5.0672182967645956</v>
+        <v>5.067218296764596</v>
       </c>
       <c r="G17">
         <v>10.92472024415056</v>
       </c>
       <c r="H17">
-        <v>52.546792066300398</v>
+        <v>52.5467920663004</v>
       </c>
       <c r="I17">
         <v>1.982214358878853</v>
       </c>
       <c r="J17">
-        <v>55.780264496439472</v>
+        <v>55.78026449643947</v>
       </c>
       <c r="K17">
-        <v>5.1058757798677714</v>
+        <v>5.105875779867771</v>
       </c>
       <c r="L17">
         <v>11.0207423580786</v>
@@ -1313,33 +1296,33 @@
         <v>1.988831104507182</v>
       </c>
       <c r="O17">
-        <v>56.562772925764193</v>
+        <v>56.56277292576419</v>
       </c>
       <c r="P17">
         <v>5.132392273402675</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18">
-        <v>17.383749999999999</v>
+        <v>17.38375</v>
       </c>
       <c r="C18">
         <v>14.00733443589559</v>
       </c>
       <c r="D18">
-        <v>1.1611418710002159</v>
+        <v>1.161141871000216</v>
       </c>
       <c r="E18">
         <v>52.36</v>
       </c>
       <c r="F18">
-        <v>3.0120083411231748</v>
+        <v>3.012008341123175</v>
       </c>
       <c r="G18">
-        <v>18.166250000000002</v>
+        <v>18.16625</v>
       </c>
       <c r="H18">
         <v>13.34204912956719</v>
@@ -1348,13 +1331,13 @@
         <v>1.157090758962362</v>
       </c>
       <c r="J18">
-        <v>54.713749999999997</v>
+        <v>54.71375</v>
       </c>
       <c r="K18">
-        <v>3.0118351338333449</v>
+        <v>3.011835133833345</v>
       </c>
       <c r="L18">
-        <v>18.054285714285719</v>
+        <v>18.05428571428572</v>
       </c>
       <c r="M18">
         <v>13.14685868017092</v>
@@ -1363,27 +1346,27 @@
         <v>1.152278841588859</v>
       </c>
       <c r="O18">
-        <v>54.496428571428567</v>
+        <v>54.49642857142857</v>
       </c>
       <c r="P18">
         <v>3.01847602468745</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19">
-        <v>38.101999999999997</v>
+        <v>38.102</v>
       </c>
       <c r="C19">
-        <v>0.16797018529211069</v>
+        <v>0.1679701852921107</v>
       </c>
       <c r="D19">
         <v>1.002519552779382</v>
       </c>
       <c r="E19">
-        <v>40.143999999999998</v>
+        <v>40.144</v>
       </c>
       <c r="F19">
         <v>1.053592987244764</v>
@@ -1392,7 +1375,7 @@
         <v>36.256</v>
       </c>
       <c r="H19">
-        <v>0.20962047661076791</v>
+        <v>0.2096204766107679</v>
       </c>
       <c r="I19">
         <v>1.003254633715799</v>
@@ -1407,36 +1390,36 @@
         <v>36.92994746059545</v>
       </c>
       <c r="M19">
-        <v>0.26556646274956142</v>
+        <v>0.2655664627495614</v>
       </c>
       <c r="N19">
-        <v>1.0040783421065109</v>
+        <v>1.004078342106511</v>
       </c>
       <c r="O19">
-        <v>39.242431823867904</v>
+        <v>39.2424318238679</v>
       </c>
       <c r="P19">
-        <v>1.0626181330406681</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1.062618133040668</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>34</v>
       </c>
       <c r="G20">
-        <v>18.261952191235061</v>
+        <v>18.26195219123506</v>
       </c>
       <c r="H20">
-        <v>0.20179983637851109</v>
+        <v>0.2017998363785111</v>
       </c>
       <c r="I20">
-        <v>1.0032724297791109</v>
+        <v>1.003272429779111</v>
       </c>
       <c r="J20">
-        <v>24.597609561752989</v>
+        <v>24.59760956175299</v>
       </c>
       <c r="K20">
-        <v>1.3469320970820839</v>
+        <v>1.346932097082084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>